<commit_message>
Fully functional version, without management. There are still certain disagreement with VBA, but to the minor extent. Getting very close
</commit_message>
<xml_diff>
--- a/dev/r3PGmix_info.xlsx
+++ b/dev/r3PGmix_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D808DFE-964B-3D49-8282-87A1F38644D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1127263C-00EC-9B49-A18D-465C79140433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="460" windowWidth="22840" windowHeight="17540" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
+    <workbookView xWindow="29200" yWindow="460" windowWidth="18020" windowHeight="28340" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
   </bookViews>
   <sheets>
     <sheet name="var_names" sheetId="1" r:id="rId1"/>
@@ -846,9 +846,6 @@
     <t>biom_stem</t>
   </si>
   <si>
-    <t>biom_total</t>
-  </si>
-  <si>
     <t>biom_tree</t>
   </si>
   <si>
@@ -942,9 +939,6 @@
     <t>epsilon_sb</t>
   </si>
   <si>
-    <t>spsilon_npp</t>
-  </si>
-  <si>
     <t>volume_incr</t>
   </si>
   <si>
@@ -972,9 +966,6 @@
     <t>litter_rate</t>
   </si>
   <si>
-    <t>biom_litter_total</t>
-  </si>
-  <si>
     <t>Self thinning</t>
   </si>
   <si>
@@ -1399,6 +1390,15 @@
   </si>
   <si>
     <t>transp_veg</t>
+  </si>
+  <si>
+    <t>var_4_4</t>
+  </si>
+  <si>
+    <t>var_4_5</t>
+  </si>
+  <si>
+    <t>epsilon_npp</t>
   </si>
 </sst>
 </file>
@@ -1752,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EDA796-FB5E-0A42-AB5E-6B438DB45270}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1791,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1871,7 +1871,7 @@
         <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F5" t="s">
         <v>189</v>
@@ -1911,13 +1911,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D7" t="s">
         <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F7" t="s">
         <v>193</v>
@@ -1995,7 +1995,7 @@
         <v>235</v>
       </c>
       <c r="H10" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>234</v>
       </c>
       <c r="H11" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2044,7 +2044,7 @@
         <v>233</v>
       </c>
       <c r="H12" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2055,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D13" t="s">
         <v>219</v>
@@ -2069,7 +2069,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D14" t="s">
         <v>219</v>
@@ -2083,7 +2083,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D15" t="s">
         <v>219</v>
@@ -2097,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D16" t="s">
         <v>219</v>
@@ -2180,7 +2180,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D20" t="s">
         <v>239</v>
@@ -2203,7 +2203,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D21" t="s">
         <v>239</v>
@@ -2226,7 +2226,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D22" t="s">
         <v>239</v>
@@ -2387,7 +2387,7 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D29" t="s">
         <v>239</v>
@@ -2401,7 +2401,7 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D30" t="s">
         <v>239</v>
@@ -2415,7 +2415,7 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D31" t="s">
         <v>239</v>
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D33" t="s">
         <v>259</v>
@@ -2507,7 +2507,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D35" t="s">
         <v>259</v>
@@ -2668,7 +2668,7 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D42" t="s">
         <v>259</v>
@@ -2682,7 +2682,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D43" t="s">
         <v>259</v>
@@ -2696,7 +2696,7 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D44" t="s">
         <v>259</v>
@@ -2710,7 +2710,7 @@
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D45" t="s">
         <v>259</v>
@@ -2724,7 +2724,7 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D46" t="s">
         <v>259</v>
@@ -2750,7 +2750,7 @@
         <v>201</v>
       </c>
       <c r="G47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2773,7 +2773,7 @@
         <v>201</v>
       </c>
       <c r="G48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2796,7 +2796,7 @@
         <v>201</v>
       </c>
       <c r="G49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>315</v>
+        <v>455</v>
       </c>
       <c r="D50" t="s">
         <v>269</v>
@@ -2819,7 +2819,7 @@
         <v>201</v>
       </c>
       <c r="G50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2830,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>273</v>
+        <v>456</v>
       </c>
       <c r="D51" t="s">
         <v>269</v>
@@ -2842,7 +2842,7 @@
         <v>201</v>
       </c>
       <c r="G51" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2853,7 +2853,7 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D52" t="s">
         <v>269</v>
@@ -2865,7 +2865,7 @@
         <v>206</v>
       </c>
       <c r="G52" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D53" t="s">
         <v>269</v>
@@ -2888,7 +2888,7 @@
         <v>207</v>
       </c>
       <c r="G53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2899,7 +2899,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D54" t="s">
         <v>269</v>
@@ -2908,7 +2908,7 @@
         <v>41</v>
       </c>
       <c r="G54" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2919,10 +2919,10 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D55" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E55" t="s">
         <v>66</v>
@@ -2931,7 +2931,7 @@
         <v>211</v>
       </c>
       <c r="G55" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H55" t="s">
         <v>156</v>
@@ -2945,10 +2945,10 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E56" t="s">
         <v>67</v>
@@ -2957,7 +2957,7 @@
         <v>201</v>
       </c>
       <c r="G56" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2968,10 +2968,10 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D57" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E57" t="s">
         <v>68</v>
@@ -2991,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D58" t="s">
         <v>269</v>
@@ -3005,7 +3005,7 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D59" t="s">
         <v>269</v>
@@ -3019,7 +3019,7 @@
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D60" t="s">
         <v>269</v>
@@ -3033,7 +3033,7 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D61" t="s">
         <v>269</v>
@@ -3047,10 +3047,10 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E62" t="s">
         <v>42</v>
@@ -3070,10 +3070,10 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E63" t="s">
         <v>43</v>
@@ -3093,10 +3093,10 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E64" t="s">
         <v>44</v>
@@ -3105,7 +3105,7 @@
         <v>200</v>
       </c>
       <c r="G64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3116,10 +3116,10 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D65" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E65" t="s">
         <v>45</v>
@@ -3139,10 +3139,10 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E66" t="s">
         <v>46</v>
@@ -3162,10 +3162,10 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E67" t="s">
         <v>47</v>
@@ -3185,10 +3185,10 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E68" t="s">
         <v>48</v>
@@ -3208,10 +3208,10 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D69" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E69" t="s">
         <v>49</v>
@@ -3231,10 +3231,10 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D70" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E70" t="s">
         <v>50</v>
@@ -3254,10 +3254,10 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D71" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E71" t="s">
         <v>51</v>
@@ -3277,10 +3277,10 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3291,10 +3291,10 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D73" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -3305,10 +3305,10 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D74" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -3319,10 +3319,10 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D75" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -3333,10 +3333,10 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D76" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -3347,10 +3347,10 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D77" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E77" t="s">
         <v>52</v>
@@ -3370,10 +3370,10 @@
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D78" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E78" t="s">
         <v>53</v>
@@ -3393,10 +3393,10 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D79" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E79" t="s">
         <v>54</v>
@@ -3405,7 +3405,7 @@
         <v>208</v>
       </c>
       <c r="G79" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -3419,7 +3419,7 @@
         <v>145</v>
       </c>
       <c r="D80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E80" t="s">
         <v>55</v>
@@ -3439,10 +3439,10 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D81" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E81" t="s">
         <v>56</v>
@@ -3462,10 +3462,10 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D82" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E82" t="s">
         <v>57</v>
@@ -3485,10 +3485,10 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D83" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E83" t="s">
         <v>58</v>
@@ -3508,10 +3508,10 @@
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>305</v>
+        <v>457</v>
       </c>
       <c r="D84" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E84" t="s">
         <v>59</v>
@@ -3531,10 +3531,10 @@
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D85" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E85" t="s">
         <v>60</v>
@@ -3554,10 +3554,10 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D86" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E86" t="s">
         <v>61</v>
@@ -3577,10 +3577,10 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D87" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E87" t="s">
         <v>62</v>
@@ -3600,10 +3600,10 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D88" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E88" t="s">
         <v>63</v>
@@ -3623,10 +3623,10 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D89" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E89" t="s">
         <v>64</v>
@@ -3646,10 +3646,10 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E90" t="s">
         <v>65</v>
@@ -3669,7 +3669,7 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -3680,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D92" t="s">
         <v>160</v>
@@ -3726,7 +3726,7 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D94" t="s">
         <v>160</v>
@@ -3738,7 +3738,7 @@
         <v>195</v>
       </c>
       <c r="G94" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -3749,7 +3749,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D95" t="s">
         <v>160</v>
@@ -3772,7 +3772,7 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D96" t="s">
         <v>160</v>
@@ -3786,7 +3786,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D97" t="s">
         <v>160</v>
@@ -3800,7 +3800,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D98" t="s">
         <v>160</v>
@@ -3814,7 +3814,7 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D99" t="s">
         <v>160</v>
@@ -3828,7 +3828,7 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D100" t="s">
         <v>160</v>
@@ -3842,7 +3842,7 @@
         <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D101" t="s">
         <v>160</v>
@@ -3856,7 +3856,7 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D102" t="s">
         <v>160</v>
@@ -3870,7 +3870,7 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D103" t="s">
         <v>160</v>
@@ -3884,7 +3884,7 @@
         <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D104" t="s">
         <v>160</v>
@@ -3898,7 +3898,7 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D105" t="s">
         <v>160</v>
@@ -3912,7 +3912,7 @@
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D106" t="s">
         <v>160</v>
@@ -3926,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D107" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E107" t="s">
         <v>74</v>
@@ -3938,7 +3938,7 @@
         <v>213</v>
       </c>
       <c r="G107" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3949,10 +3949,10 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D108" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E108" t="s">
         <v>75</v>
@@ -3961,7 +3961,7 @@
         <v>213</v>
       </c>
       <c r="G108" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3972,10 +3972,10 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D109" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E109" t="s">
         <v>76</v>
@@ -3984,7 +3984,7 @@
         <v>200</v>
       </c>
       <c r="G109" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H109" t="s">
         <v>161</v>
@@ -3998,10 +3998,10 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D110" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E110" t="s">
         <v>77</v>
@@ -4010,7 +4010,7 @@
         <v>213</v>
       </c>
       <c r="G110" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H110" t="s">
         <v>162</v>
@@ -4024,10 +4024,10 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D111" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E111" t="s">
         <v>78</v>
@@ -4047,10 +4047,10 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D112" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E112" t="s">
         <v>79</v>
@@ -4070,10 +4070,10 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D113" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E113" t="s">
         <v>80</v>
@@ -4082,7 +4082,7 @@
         <v>215</v>
       </c>
       <c r="G113" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -4093,10 +4093,10 @@
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D114" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E114" t="s">
         <v>81</v>
@@ -4116,10 +4116,10 @@
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D115" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E115" t="s">
         <v>82</v>
@@ -4139,10 +4139,10 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D116" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E116" t="s">
         <v>83</v>
@@ -4151,7 +4151,7 @@
         <v>215</v>
       </c>
       <c r="G116" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -4162,10 +4162,10 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D117" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E117" t="s">
         <v>84</v>
@@ -4174,10 +4174,10 @@
         <v>215</v>
       </c>
       <c r="G117" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I117" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -4188,10 +4188,10 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D118" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E118" t="s">
         <v>85</v>
@@ -4211,10 +4211,10 @@
         <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D119" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E119" t="s">
         <v>86</v>
@@ -4223,7 +4223,7 @@
         <v>213</v>
       </c>
       <c r="G119" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -4234,10 +4234,10 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D120" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -4248,10 +4248,10 @@
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D121" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -4262,10 +4262,10 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D122" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E122" t="s">
         <v>87</v>
@@ -4285,10 +4285,10 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D123" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E123" t="s">
         <v>88</v>
@@ -4308,10 +4308,10 @@
         <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D124" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E124" t="s">
         <v>89</v>
@@ -4331,10 +4331,10 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D125" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E125" t="s">
         <v>90</v>
@@ -4354,10 +4354,10 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D126" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E126" t="s">
         <v>91</v>
@@ -4377,10 +4377,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D127" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E127" t="s">
         <v>92</v>
@@ -4400,10 +4400,10 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D128" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E128" t="s">
         <v>93</v>
@@ -4423,10 +4423,10 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D129" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E129" t="s">
         <v>94</v>
@@ -4446,10 +4446,10 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D130" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E130" t="s">
         <v>95</v>
@@ -4469,10 +4469,10 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D131" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -4483,10 +4483,10 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D132" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -4497,10 +4497,10 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D133" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -4511,10 +4511,10 @@
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D134" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -4525,10 +4525,10 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D135" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4539,10 +4539,10 @@
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D136" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4553,10 +4553,10 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D137" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E137" t="s">
         <v>96</v>
@@ -4565,7 +4565,7 @@
         <v>200</v>
       </c>
       <c r="G137" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H137" t="s">
         <v>175</v>
@@ -4579,10 +4579,10 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D138" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E138" t="s">
         <v>97</v>
@@ -4591,7 +4591,7 @@
         <v>200</v>
       </c>
       <c r="G138" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H138" t="s">
         <v>176</v>
@@ -4605,10 +4605,10 @@
         <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D139" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E139" t="s">
         <v>98</v>
@@ -4617,7 +4617,7 @@
         <v>200</v>
       </c>
       <c r="G139" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H139" t="s">
         <v>177</v>
@@ -4631,10 +4631,10 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D140" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E140" t="s">
         <v>99</v>
@@ -4643,7 +4643,7 @@
         <v>200</v>
       </c>
       <c r="G140" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H140" t="s">
         <v>178</v>
@@ -4657,10 +4657,10 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D141" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E141" t="s">
         <v>100</v>
@@ -4669,7 +4669,7 @@
         <v>200</v>
       </c>
       <c r="G141" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H141" t="s">
         <v>179</v>
@@ -4683,10 +4683,10 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D142" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E142" t="s">
         <v>101</v>
@@ -4695,7 +4695,7 @@
         <v>200</v>
       </c>
       <c r="G142" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H142" t="s">
         <v>180</v>
@@ -4709,10 +4709,10 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D143" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E143" t="s">
         <v>102</v>
@@ -4721,7 +4721,7 @@
         <v>204</v>
       </c>
       <c r="G143" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H143" t="s">
         <v>181</v>
@@ -4735,10 +4735,10 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D144" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E144" t="s">
         <v>103</v>
@@ -4747,7 +4747,7 @@
         <v>204</v>
       </c>
       <c r="G144" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H144" t="s">
         <v>182</v>
@@ -4761,10 +4761,10 @@
         <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D145" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E145" t="s">
         <v>104</v>
@@ -4773,7 +4773,7 @@
         <v>204</v>
       </c>
       <c r="G145" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H145" t="s">
         <v>183</v>
@@ -4787,10 +4787,10 @@
         <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D146" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E146" t="s">
         <v>105</v>
@@ -4799,7 +4799,7 @@
         <v>204</v>
       </c>
       <c r="G146" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H146" t="s">
         <v>184</v>
@@ -4813,10 +4813,10 @@
         <v>11</v>
       </c>
       <c r="C147" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D147" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E147" t="s">
         <v>106</v>
@@ -4825,7 +4825,7 @@
         <v>204</v>
       </c>
       <c r="G147" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H147" t="s">
         <v>185</v>
@@ -4839,10 +4839,10 @@
         <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D148" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E148" t="s">
         <v>107</v>
@@ -4851,7 +4851,7 @@
         <v>204</v>
       </c>
       <c r="G148" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H148" t="s">
         <v>186</v>
@@ -4865,10 +4865,10 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D149" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E149" t="s">
         <v>108</v>
@@ -4877,7 +4877,7 @@
         <v>204</v>
       </c>
       <c r="G149" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H149" t="s">
         <v>187</v>
@@ -4891,10 +4891,10 @@
         <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D150" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E150" t="s">
         <v>109</v>
@@ -4903,7 +4903,7 @@
         <v>204</v>
       </c>
       <c r="G150" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H150" t="s">
         <v>188</v>
@@ -4917,10 +4917,10 @@
         <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D151" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4931,10 +4931,10 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D152" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E152" t="s">
         <v>23</v>
@@ -4943,7 +4943,7 @@
         <v>195</v>
       </c>
       <c r="G152" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H152" t="s">
         <v>119</v>
@@ -4957,10 +4957,10 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D153" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E153" t="s">
         <v>17</v>
@@ -4969,7 +4969,7 @@
         <v>198</v>
       </c>
       <c r="G153" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H153" t="s">
         <v>120</v>
@@ -4983,10 +4983,10 @@
         <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D154" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E154" t="s">
         <v>12</v>
@@ -4995,7 +4995,7 @@
         <v>196</v>
       </c>
       <c r="G154" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H154" t="s">
         <v>121</v>
@@ -5009,10 +5009,10 @@
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D155" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E155" t="s">
         <v>13</v>
@@ -5021,7 +5021,7 @@
         <v>197</v>
       </c>
       <c r="G155" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H155" t="s">
         <v>122</v>
@@ -5035,10 +5035,10 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D156" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E156" t="s">
         <v>19</v>
@@ -5047,7 +5047,7 @@
         <v>151</v>
       </c>
       <c r="G156" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="H156" t="s">
         <v>123</v>
@@ -5061,10 +5061,10 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D157" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E157" t="s">
         <v>24</v>
@@ -5073,7 +5073,7 @@
         <v>201</v>
       </c>
       <c r="G157" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H157" t="s">
         <v>124</v>
@@ -5087,10 +5087,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D158" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -5101,10 +5101,10 @@
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D159" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -5115,10 +5115,10 @@
         <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D160" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5129,10 +5129,10 @@
         <v>10</v>
       </c>
       <c r="C161" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D161" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -5143,10 +5143,10 @@
         <v>11</v>
       </c>
       <c r="C162" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D162" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -5157,10 +5157,10 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D163" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -5171,10 +5171,10 @@
         <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D164" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -5185,10 +5185,10 @@
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D165" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -5199,10 +5199,10 @@
         <v>15</v>
       </c>
       <c r="C166" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D166" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Stand` variables are done!
</commit_message>
<xml_diff>
--- a/dev/r3PGmix_info.xlsx
+++ b/dev/r3PGmix_info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F68FE-2FD1-DB40-9D0A-9822DE42E821}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACC7F63-5428-5442-A241-49493EB1D0FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27280" yWindow="460" windowWidth="18020" windowHeight="28340" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
+    <workbookView xWindow="28180" yWindow="460" windowWidth="18020" windowHeight="28340" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
   </bookViews>
   <sheets>
     <sheet name="var_names" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="447">
   <si>
     <t>description</t>
   </si>
@@ -66,15 +67,6 @@
     <t>Stand volume excluding branch &amp; bark</t>
   </si>
   <si>
-    <t>Cumulative extracted volume (by thinning)</t>
-  </si>
-  <si>
-    <t>Total cumulative volume (stand volume + extracted volume +  mortality)</t>
-  </si>
-  <si>
-    <t>Volume extracted during the most recent thinning event</t>
-  </si>
-  <si>
     <t>Mean DBH</t>
   </si>
   <si>
@@ -753,30 +745,9 @@
     <t>Basal area</t>
   </si>
   <si>
-    <t>volume_stand</t>
-  </si>
-  <si>
     <t>Stand volume</t>
   </si>
   <si>
-    <t>volume_extract</t>
-  </si>
-  <si>
-    <t>Extracted volume</t>
-  </si>
-  <si>
-    <t>volume_cumul</t>
-  </si>
-  <si>
-    <t>Total cumulative volume</t>
-  </si>
-  <si>
-    <t>volume_extract_last</t>
-  </si>
-  <si>
-    <t>Latest extracted volume</t>
-  </si>
-  <si>
     <t>volume_mai</t>
   </si>
   <si>
@@ -1384,6 +1355,18 @@
   </si>
   <si>
     <t>var_1_11</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>var_2_10</t>
+  </si>
+  <si>
+    <t>var_2_11</t>
+  </si>
+  <si>
+    <t>var_2_12</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1721,7 @@
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1755,13 +1738,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1776,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1787,16 +1770,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1807,16 +1790,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1827,19 +1810,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G4" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1850,19 +1833,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="F5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G5" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1873,19 +1856,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G6" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1896,19 +1879,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1919,19 +1902,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1942,19 +1925,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1965,16 +1948,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1985,19 +1968,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2008,10 +1991,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="D12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2022,10 +2005,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2036,10 +2019,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2050,10 +2033,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2064,10 +2047,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2078,19 +2061,19 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17" t="s">
+        <v>233</v>
+      </c>
+      <c r="G17" t="s">
         <v>234</v>
-      </c>
-      <c r="D17" t="s">
-        <v>233</v>
-      </c>
-      <c r="E17" t="s">
-        <v>235</v>
-      </c>
-      <c r="F17" t="s">
-        <v>236</v>
-      </c>
-      <c r="G17" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2101,19 +2084,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2124,19 +2107,19 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G19" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2147,19 +2130,19 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="D20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2170,19 +2153,19 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2193,19 +2176,19 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="D22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2216,19 +2199,19 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G23" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2239,19 +2222,19 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
+        <v>443</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G24" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2262,19 +2245,19 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2285,19 +2268,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>246</v>
+        <v>444</v>
       </c>
       <c r="D26" t="s">
-        <v>233</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" t="s">
-        <v>193</v>
-      </c>
-      <c r="G26" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2308,19 +2282,10 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>248</v>
+        <v>445</v>
       </c>
       <c r="D27" t="s">
-        <v>233</v>
-      </c>
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" t="s">
-        <v>193</v>
-      </c>
-      <c r="G27" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2331,19 +2296,10 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>250</v>
+        <v>446</v>
       </c>
       <c r="D28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" t="s">
-        <v>195</v>
-      </c>
-      <c r="G28" t="s">
-        <v>111</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2354,10 +2310,10 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D29" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -2368,10 +2324,10 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2382,19 +2338,10 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="D31" t="s">
-        <v>233</v>
-      </c>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" t="s">
-        <v>196</v>
-      </c>
-      <c r="G31" t="s">
-        <v>114</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2405,19 +2352,19 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D32" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2428,19 +2375,19 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D33" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G33" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -2451,19 +2398,19 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D34" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F34" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2474,19 +2421,19 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D35" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2497,19 +2444,19 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D36" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2520,19 +2467,19 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D37" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2543,19 +2490,19 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D38" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G38" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2566,19 +2513,19 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D39" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G39" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2589,19 +2536,19 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D40" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G40" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2612,19 +2559,19 @@
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D41" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F41" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2635,10 +2582,10 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D42" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2649,10 +2596,10 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="D43" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2663,10 +2610,10 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D44" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2677,10 +2624,10 @@
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="D45" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2691,10 +2638,10 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D46" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2705,19 +2652,19 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D47" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G47" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2728,19 +2675,19 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D48" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E48" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F48" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G48" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2751,19 +2698,19 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D49" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E49" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G49" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2774,19 +2721,19 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D50" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E50" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F50" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G50" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2797,19 +2744,19 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D51" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F51" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G51" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2820,19 +2767,19 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D52" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E52" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G52" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2843,19 +2790,19 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D53" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E53" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G53" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2866,16 +2813,16 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D54" t="s">
+        <v>253</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" t="s">
         <v>263</v>
-      </c>
-      <c r="E54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G54" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2886,22 +2833,22 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D55" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G55" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="H55" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2912,19 +2859,19 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="D56" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E56" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F56" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G56" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2935,19 +2882,19 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="D57" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F57" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G57" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2958,10 +2905,10 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="D58" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2972,10 +2919,10 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D59" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2986,10 +2933,10 @@
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="D60" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -3000,10 +2947,10 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D61" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -3014,19 +2961,19 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D62" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E62" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F62" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G62" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -3037,19 +2984,19 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D63" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E63" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F63" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G63" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -3060,19 +3007,19 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D64" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F64" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G64" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3083,19 +3030,19 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D65" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E65" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G65" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -3106,19 +3053,19 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D66" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E66" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F66" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G66" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -3129,19 +3076,19 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D67" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E67" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G67" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -3152,19 +3099,19 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D68" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E68" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F68" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -3175,19 +3122,19 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D69" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G69" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -3198,19 +3145,19 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D70" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E70" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F70" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G70" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -3221,19 +3168,19 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D71" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="E71" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F71" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -3244,10 +3191,10 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="D72" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3258,10 +3205,10 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="D73" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -3272,10 +3219,10 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D74" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -3286,10 +3233,10 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="D75" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -3300,10 +3247,10 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="D76" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -3314,19 +3261,19 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D77" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E77" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F77" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G77" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -3337,19 +3284,19 @@
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D78" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E78" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F78" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G78" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -3360,19 +3307,19 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D79" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E79" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F79" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G79" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -3383,19 +3330,19 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D80" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E80" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F80" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G80" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -3406,19 +3353,19 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D81" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E81" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F81" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G81" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -3429,19 +3376,19 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="D82" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E82" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F82" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G82" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -3452,19 +3399,19 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D83" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E83" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F83" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G83" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -3475,19 +3422,19 @@
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D84" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E84" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -3498,19 +3445,19 @@
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D85" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E85" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F85" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G85" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -3521,19 +3468,19 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D86" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E86" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F86" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G86" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -3544,19 +3491,19 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="D87" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E87" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F87" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G87" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -3567,19 +3514,19 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="D88" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E88" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F88" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G88" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3590,19 +3537,19 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="D89" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E89" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F89" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G89" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -3613,19 +3560,19 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D90" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E90" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F90" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G90" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -3636,10 +3583,10 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="D91" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -3650,19 +3597,19 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="D92" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E92" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F92" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G92" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -3673,19 +3620,19 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D93" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E93" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F93" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G93" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3696,19 +3643,19 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D94" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E94" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F94" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G94" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -3719,19 +3666,19 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D95" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E95" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G95" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -3742,10 +3689,10 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D96" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3756,10 +3703,10 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D97" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3770,10 +3717,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D98" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3784,10 +3731,10 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D99" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3798,10 +3745,10 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="D100" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3812,10 +3759,10 @@
         <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="D101" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3826,10 +3773,10 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="D102" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3840,10 +3787,10 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="D103" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3854,10 +3801,10 @@
         <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="D104" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3868,10 +3815,10 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D105" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3882,10 +3829,10 @@
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D106" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3896,19 +3843,19 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D107" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E107" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F107" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G107" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3919,19 +3866,19 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D108" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E108" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F108" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G108" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3942,22 +3889,22 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D109" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E109" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F109" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G109" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="H109" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3968,22 +3915,22 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D110" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E110" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F110" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G110" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="H110" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3994,19 +3941,19 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D111" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E111" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F111" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G111" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -4017,19 +3964,19 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D112" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E112" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F112" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G112" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
@@ -4040,19 +3987,19 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="D113" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E113" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F113" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G113" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -4063,19 +4010,19 @@
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D114" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E114" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F114" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G114" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -4086,19 +4033,19 @@
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="D115" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E115" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F115" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G115" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -4109,19 +4056,19 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="D116" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E116" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F116" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G116" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -4132,22 +4079,22 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="D117" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E117" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F117" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G117" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="I117" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -4158,19 +4105,19 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D118" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E118" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F118" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G118" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -4181,19 +4128,19 @@
         <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D119" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E119" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F119" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G119" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -4204,10 +4151,10 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="D120" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -4218,10 +4165,10 @@
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D121" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -4232,19 +4179,19 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D122" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E122" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F122" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G122" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -4255,19 +4202,19 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="D123" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E123" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F123" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G123" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -4278,19 +4225,19 @@
         <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D124" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E124" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F124" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G124" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -4301,19 +4248,19 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D125" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E125" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F125" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G125" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -4324,19 +4271,19 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="D126" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E126" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F126" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G126" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -4347,19 +4294,19 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="D127" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E127" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F127" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G127" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -4370,19 +4317,19 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D128" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E128" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F128" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G128" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -4393,19 +4340,19 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="D129" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E129" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F129" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G129" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -4416,19 +4363,19 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D130" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E130" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F130" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G130" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -4439,10 +4386,10 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="D131" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -4453,10 +4400,10 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="D132" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -4467,10 +4414,10 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="D133" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -4481,10 +4428,10 @@
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D134" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -4495,10 +4442,10 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="D135" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4509,10 +4456,10 @@
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="D136" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4523,22 +4470,22 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="D137" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E137" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F137" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G137" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="H137" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -4549,22 +4496,22 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D138" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E138" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F138" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G138" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="H138" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -4575,22 +4522,22 @@
         <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D139" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E139" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F139" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G139" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="H139" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -4601,22 +4548,22 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D140" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E140" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F140" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G140" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="H140" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4627,22 +4574,22 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D141" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E141" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F141" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G141" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="H141" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4653,22 +4600,22 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D142" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E142" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F142" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G142" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="H142" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4679,22 +4626,22 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D143" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E143" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F143" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G143" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="H143" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4705,22 +4652,22 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D144" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E144" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F144" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G144" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="H144" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -4731,22 +4678,22 @@
         <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="D145" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E145" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F145" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G145" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="H145" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -4757,22 +4704,22 @@
         <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="D146" t="s">
+        <v>323</v>
+      </c>
+      <c r="E146" t="s">
+        <v>101</v>
+      </c>
+      <c r="F146" t="s">
+        <v>197</v>
+      </c>
+      <c r="G146" t="s">
         <v>333</v>
       </c>
-      <c r="E146" t="s">
-        <v>104</v>
-      </c>
-      <c r="F146" t="s">
-        <v>200</v>
-      </c>
-      <c r="G146" t="s">
-        <v>343</v>
-      </c>
       <c r="H146" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -4783,22 +4730,22 @@
         <v>11</v>
       </c>
       <c r="C147" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D147" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E147" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F147" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G147" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="H147" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -4809,22 +4756,22 @@
         <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="D148" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E148" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F148" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G148" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="H148" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -4835,22 +4782,22 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D149" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E149" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F149" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G149" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="H149" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -4861,22 +4808,22 @@
         <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D150" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E150" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F150" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G150" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="H150" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4887,10 +4834,10 @@
         <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="D151" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4901,22 +4848,22 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="D152" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E152" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F152" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G152" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="H152" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -4927,22 +4874,22 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="D153" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E153" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F153" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G153" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="H153" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -4953,22 +4900,22 @@
         <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D154" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E154" t="s">
         <v>11</v>
       </c>
       <c r="F154" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G154" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="H154" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -4979,22 +4926,22 @@
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="D155" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E155" t="s">
         <v>12</v>
       </c>
       <c r="F155" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G155" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="H155" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -5005,22 +4952,22 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D156" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E156" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F156" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G156" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="H156" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -5031,22 +4978,22 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="D157" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="E157" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F157" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G157" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="H157" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -5057,10 +5004,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D158" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -5071,10 +5018,10 @@
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="D159" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -5085,10 +5032,10 @@
         <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="D160" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5099,10 +5046,10 @@
         <v>10</v>
       </c>
       <c r="C161" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="D161" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -5113,10 +5060,10 @@
         <v>11</v>
       </c>
       <c r="C162" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="D162" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -5127,10 +5074,10 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="D163" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -5141,10 +5088,10 @@
         <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="D164" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -5155,10 +5102,10 @@
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="D165" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -5169,10 +5116,316 @@
         <v>15</v>
       </c>
       <c r="C166" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="D166" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12872662-7795-8E49-8B63-4C56A42E1535}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>363</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>370</v>
+      </c>
+      <c r="D15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I found the 'issue' which let to mismatch with David version. It was related to how basal area is calculated. Within David's version he use not biass corrected basal area which lead to discrepansies.
</commit_message>
<xml_diff>
--- a/dev/r3PGmix_info.xlsx
+++ b/dev/r3PGmix_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACC7F63-5428-5442-A241-49493EB1D0FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19351E6-E4F6-9B4F-A50E-4DFCC729D947}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28180" yWindow="460" windowWidth="18020" windowHeight="28340" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="405">
   <si>
     <t>description</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Mean crown diameter</t>
   </si>
   <si>
-    <t>Mean individual tree leaf area to crown surface area ratio</t>
-  </si>
-  <si>
     <t>Number of crop trees (x)</t>
   </si>
   <si>
@@ -127,12 +124,6 @@
     <t>Root biomass</t>
   </si>
   <si>
-    <t>Accumulated litterfall</t>
-  </si>
-  <si>
-    <t>Total biomass</t>
-  </si>
-  <si>
     <t>Mean stem biomass per tree</t>
   </si>
   <si>
@@ -190,18 +181,6 @@
     <t>Light-use efficiency based on GPP</t>
   </si>
   <si>
-    <t>Light-use efficiency based on stem biomass (increment in WS)</t>
-  </si>
-  <si>
-    <t>Light-use efficiency based on NPP</t>
-  </si>
-  <si>
-    <t>Stem volume increment in current period</t>
-  </si>
-  <si>
-    <t>FR modifier of root biomass allocation</t>
-  </si>
-  <si>
     <t>Fraction of NPP allocated to roots</t>
   </si>
   <si>
@@ -214,15 +193,9 @@
     <t>Ratio of foliage to stem biomass allocation</t>
   </si>
   <si>
-    <t>Current leaf litterfall rate</t>
-  </si>
-  <si>
     <t>Litter fall in current period</t>
   </si>
   <si>
-    <t>The NPP that must be assimilated before further any growth (for decidous species)</t>
-  </si>
-  <si>
     <t>Stem mortality</t>
   </si>
   <si>
@@ -292,18 +265,6 @@
     <t>Inter-cellular CO2 concentration</t>
   </si>
   <si>
-    <t>The ratio of diffusivities of CO2 and water vapor in air</t>
-  </si>
-  <si>
-    <t>d13C difference of modeled tissue and new photosynthate</t>
-  </si>
-  <si>
-    <t>Fractionation again 13C in diffusion</t>
-  </si>
-  <si>
-    <t>Enzymatic fractionation by Rubisco</t>
-  </si>
-  <si>
     <t>Weibull scale parameter of avDBH distribution</t>
   </si>
   <si>
@@ -361,9 +322,6 @@
     <t>LCL</t>
   </si>
   <si>
-    <t>treeLAtoSAratio</t>
-  </si>
-  <si>
     <t>CropTrees</t>
   </si>
   <si>
@@ -451,15 +409,6 @@
     <t>Epsilon</t>
   </si>
   <si>
-    <t>StemEpsilon</t>
-  </si>
-  <si>
-    <t>NPPEpsilon</t>
-  </si>
-  <si>
-    <t>CVI</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -475,12 +424,6 @@
     <t>pFS</t>
   </si>
   <si>
-    <t>gammaF</t>
-  </si>
-  <si>
-    <t>NPPdebt</t>
-  </si>
-  <si>
     <t>wSmax</t>
   </si>
   <si>
@@ -520,18 +463,6 @@
     <t>InterCiPPM</t>
   </si>
   <si>
-    <t>RGcGW</t>
-  </si>
-  <si>
-    <t>D13CTissueDif</t>
-  </si>
-  <si>
-    <t>aFracDiffu</t>
-  </si>
-  <si>
-    <t>bFracRubi</t>
-  </si>
-  <si>
     <t>Dweibullscale</t>
   </si>
   <si>
@@ -769,9 +700,6 @@
     <t>lai</t>
   </si>
   <si>
-    <t>layer</t>
-  </si>
-  <si>
     <t>lai_above</t>
   </si>
   <si>
@@ -805,12 +733,6 @@
     <t>wood_density</t>
   </si>
   <si>
-    <t>Total litter</t>
-  </si>
-  <si>
-    <t>Total DM</t>
-  </si>
-  <si>
     <t>Mean stem mass</t>
   </si>
   <si>
@@ -829,9 +751,6 @@
     <t>Root DM</t>
   </si>
   <si>
-    <t>biom_bb_fract</t>
-  </si>
-  <si>
     <t>canopy_vol_frac</t>
   </si>
   <si>
@@ -889,21 +808,9 @@
     <t>epsilon_gpp</t>
   </si>
   <si>
-    <t>epsilon_sb</t>
-  </si>
-  <si>
-    <t>volume_incr</t>
-  </si>
-  <si>
-    <t>Litter fall rate</t>
-  </si>
-  <si>
     <t>Litter fall</t>
   </si>
   <si>
-    <t>f_biom_root</t>
-  </si>
-  <si>
     <t>npp_fract_root</t>
   </si>
   <si>
@@ -913,12 +820,6 @@
     <t>npp_fract_foliage</t>
   </si>
   <si>
-    <t>npp_foliage_stem_rat</t>
-  </si>
-  <si>
-    <t>litter_rate</t>
-  </si>
-  <si>
     <t>Self thinning</t>
   </si>
   <si>
@@ -982,9 +883,6 @@
     <t>wue_transp</t>
   </si>
   <si>
-    <t>transp</t>
-  </si>
-  <si>
     <t>asw</t>
   </si>
   <si>
@@ -1042,48 +940,6 @@
     <t>Relative bias in crown diameter from using mean dbh</t>
   </si>
   <si>
-    <t>weib_scale_dbh</t>
-  </si>
-  <si>
-    <t>weib_shape_dbh</t>
-  </si>
-  <si>
-    <t>weib_locat_dbh</t>
-  </si>
-  <si>
-    <t>weib_scale_biomas</t>
-  </si>
-  <si>
-    <t>weib_shape_biomas</t>
-  </si>
-  <si>
-    <t>weib_locat_biomas</t>
-  </si>
-  <si>
-    <t>bias_rel_biomas</t>
-  </si>
-  <si>
-    <t>bias_rel_dbh_pfs</t>
-  </si>
-  <si>
-    <t>bias_rel_dbh_heigh</t>
-  </si>
-  <si>
-    <t>bias_rel_dbh_ba</t>
-  </si>
-  <si>
-    <t>bias_rel_dbh_cd</t>
-  </si>
-  <si>
-    <t>bias_rel_dbh_cl</t>
-  </si>
-  <si>
-    <t>cv_biomass</t>
-  </si>
-  <si>
-    <t>slope_cv_dbh_age</t>
-  </si>
-  <si>
     <t>crop_trees</t>
   </si>
   <si>
@@ -1141,9 +997,6 @@
     <t>var_2_15</t>
   </si>
   <si>
-    <t>var_3_2</t>
-  </si>
-  <si>
     <t>var_3_11</t>
   </si>
   <si>
@@ -1306,9 +1159,6 @@
     <t>var_6_15</t>
   </si>
   <si>
-    <t>biom_foliage_debt</t>
-  </si>
-  <si>
     <t>evapo_transp</t>
   </si>
   <si>
@@ -1327,15 +1177,6 @@
     <t>transp_veg</t>
   </si>
   <si>
-    <t>var_4_4</t>
-  </si>
-  <si>
-    <t>var_4_5</t>
-  </si>
-  <si>
-    <t>epsilon_npp</t>
-  </si>
-  <si>
     <t>Gc_mol</t>
   </si>
   <si>
@@ -1367,6 +1208,39 @@
   </si>
   <si>
     <t>var_2_12</t>
+  </si>
+  <si>
+    <t>canopy_cover</t>
+  </si>
+  <si>
+    <t>layer_id</t>
+  </si>
+  <si>
+    <t>var_4_10</t>
+  </si>
+  <si>
+    <t>var_4_11</t>
+  </si>
+  <si>
+    <t>var_4_8</t>
+  </si>
+  <si>
+    <t>var_4_9</t>
+  </si>
+  <si>
+    <t>fracBB</t>
+  </si>
+  <si>
+    <t>var_6_14</t>
+  </si>
+  <si>
+    <t>var_6_12</t>
+  </si>
+  <si>
+    <t>var_6_13</t>
+  </si>
+  <si>
+    <t>var_6_11</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EDA796-FB5E-0A42-AB5E-6B438DB45270}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,13 +1612,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1759,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>362</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1770,16 +1644,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E2" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1790,16 +1664,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1810,19 +1684,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="G4" t="s">
-        <v>441</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1833,19 +1707,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>439</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1856,19 +1730,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="G6" t="s">
-        <v>440</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1879,19 +1753,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>359</v>
+        <v>311</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E7" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="G7" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1902,19 +1776,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D8" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1925,19 +1799,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1948,16 +1822,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1968,19 +1842,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="G11" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1991,10 +1865,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2005,10 +1879,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>364</v>
+        <v>316</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2019,10 +1893,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>365</v>
+        <v>317</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2033,10 +1907,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2047,10 +1921,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2061,19 +1935,19 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="F17" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="G17" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2084,19 +1958,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="G18" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2107,19 +1981,19 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="D19" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="G19" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2130,16 +2004,16 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>429</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -2153,19 +2027,19 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2176,19 +2050,19 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="D22" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2199,19 +2073,19 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="D23" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2222,19 +2096,19 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
       <c r="D24" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="G24" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2245,19 +2119,19 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="D25" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E25" t="s">
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="G25" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2268,10 +2142,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
       <c r="D26" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2282,10 +2156,10 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>445</v>
+        <v>392</v>
       </c>
       <c r="D27" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2296,10 +2170,10 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>446</v>
+        <v>393</v>
       </c>
       <c r="D28" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2310,10 +2184,10 @@
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>368</v>
+        <v>320</v>
       </c>
       <c r="D29" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -2324,10 +2198,10 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -2338,10 +2212,10 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>370</v>
+        <v>322</v>
       </c>
       <c r="D31" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -2352,19 +2226,19 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="D32" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -2375,19 +2249,19 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G33" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -2398,19 +2272,19 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D34" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2421,19 +2295,19 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="D35" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F35" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G35" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2444,19 +2318,19 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>395</v>
       </c>
       <c r="D36" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G36" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2467,19 +2341,19 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="D37" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="G37" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2490,19 +2364,19 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D38" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G38" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2513,19 +2387,19 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="D39" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G39" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2536,19 +2410,19 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D40" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F40" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="G40" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2559,19 +2433,19 @@
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="D41" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="G41" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2582,10 +2456,10 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>372</v>
+        <v>323</v>
       </c>
       <c r="D42" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2596,10 +2470,10 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>373</v>
+        <v>324</v>
       </c>
       <c r="D43" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2610,10 +2484,10 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>374</v>
+        <v>325</v>
       </c>
       <c r="D44" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2624,10 +2498,10 @@
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>375</v>
+        <v>326</v>
       </c>
       <c r="D45" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2638,10 +2512,10 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>376</v>
+        <v>327</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2652,19 +2526,19 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="D47" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E47" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G47" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2675,22 +2549,22 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="D48" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F48" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G48" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>4</v>
       </c>
@@ -2698,22 +2572,22 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="D49" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E49" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F49" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G49" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2721,22 +2595,22 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>433</v>
+        <v>233</v>
       </c>
       <c r="D50" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F50" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="G50" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2744,22 +2618,22 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>434</v>
+        <v>234</v>
       </c>
       <c r="D51" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F51" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="G51" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>4</v>
       </c>
@@ -2767,22 +2641,19 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>257</v>
+        <v>400</v>
       </c>
       <c r="D52" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E52" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" t="s">
-        <v>199</v>
+        <v>34</v>
       </c>
       <c r="G52" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>4</v>
       </c>
@@ -2790,22 +2661,22 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>258</v>
+        <v>381</v>
       </c>
       <c r="D53" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="E53" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="F53" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="G53" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>4</v>
       </c>
@@ -2813,19 +2684,13 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>267</v>
+        <v>398</v>
       </c>
       <c r="D54" t="s">
-        <v>253</v>
-      </c>
-      <c r="E54" t="s">
-        <v>37</v>
-      </c>
-      <c r="G54" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4</v>
       </c>
@@ -2833,25 +2698,13 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>296</v>
+        <v>399</v>
       </c>
       <c r="D55" t="s">
-        <v>253</v>
-      </c>
-      <c r="E55" t="s">
-        <v>62</v>
-      </c>
-      <c r="F55" t="s">
-        <v>204</v>
-      </c>
-      <c r="G55" t="s">
-        <v>289</v>
-      </c>
-      <c r="H55" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>4</v>
       </c>
@@ -2859,22 +2712,13 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>431</v>
+        <v>396</v>
       </c>
       <c r="D56" t="s">
-        <v>253</v>
-      </c>
-      <c r="E56" t="s">
-        <v>63</v>
-      </c>
-      <c r="F56" t="s">
-        <v>194</v>
-      </c>
-      <c r="G56" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>4</v>
       </c>
@@ -2882,22 +2726,13 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>426</v>
+        <v>397</v>
       </c>
       <c r="D57" t="s">
-        <v>253</v>
-      </c>
-      <c r="E57" t="s">
-        <v>64</v>
-      </c>
-      <c r="F57" t="s">
-        <v>194</v>
-      </c>
-      <c r="G57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>4</v>
       </c>
@@ -2905,13 +2740,13 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>377</v>
+        <v>328</v>
       </c>
       <c r="D58" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>4</v>
       </c>
@@ -2919,13 +2754,13 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>378</v>
+        <v>329</v>
       </c>
       <c r="D59" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>4</v>
       </c>
@@ -2933,13 +2768,13 @@
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>379</v>
+        <v>330</v>
       </c>
       <c r="D60" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>4</v>
       </c>
@@ -2947,13 +2782,13 @@
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>380</v>
+        <v>331</v>
       </c>
       <c r="D61" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>5</v>
       </c>
@@ -2961,22 +2796,22 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="D62" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E62" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F62" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G62" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5</v>
       </c>
@@ -2984,22 +2819,22 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="D63" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F63" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>5</v>
       </c>
@@ -3007,19 +2842,19 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="D64" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E64" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F64" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G64" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -3030,19 +2865,19 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="D65" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E65" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F65" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G65" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -3053,19 +2888,19 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="D66" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E66" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F66" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G66" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -3076,19 +2911,19 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="D67" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F67" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G67" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -3099,19 +2934,19 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>277</v>
+        <v>250</v>
       </c>
       <c r="D68" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F68" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G68" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -3122,19 +2957,19 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
       <c r="D69" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E69" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F69" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G69" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -3145,19 +2980,19 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="D70" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E70" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G70" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -3168,19 +3003,19 @@
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="D71" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="E71" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F71" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G71" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -3191,10 +3026,10 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>381</v>
+        <v>332</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3205,10 +3040,10 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>382</v>
+        <v>333</v>
       </c>
       <c r="D73" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -3219,10 +3054,10 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>383</v>
+        <v>334</v>
       </c>
       <c r="D74" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -3233,10 +3068,10 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="D75" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -3247,10 +3082,10 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>385</v>
+        <v>336</v>
       </c>
       <c r="D76" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -3261,19 +3096,19 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="D77" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E77" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G77" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -3284,19 +3119,19 @@
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="D78" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E78" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G78" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -3307,19 +3142,19 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="D79" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E79" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F79" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="G79" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -3330,19 +3165,19 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D80" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E80" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G80" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -3353,19 +3188,19 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>285</v>
+        <v>258</v>
       </c>
       <c r="D81" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E81" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F81" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="G81" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -3376,19 +3211,19 @@
         <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E82" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F82" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="G82" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -3399,19 +3234,19 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="D83" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E83" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F83" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="G83" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -3422,19 +3257,19 @@
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>435</v>
+        <v>263</v>
       </c>
       <c r="D84" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F84" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="G84" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -3445,19 +3280,19 @@
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="D85" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E85" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F85" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="G85" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -3468,19 +3303,19 @@
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>291</v>
+        <v>131</v>
       </c>
       <c r="D86" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="E86" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F86" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G86" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -3491,19 +3326,10 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>292</v>
+        <v>404</v>
       </c>
       <c r="D87" t="s">
-        <v>281</v>
-      </c>
-      <c r="E87" t="s">
-        <v>58</v>
-      </c>
-      <c r="F87" t="s">
-        <v>193</v>
-      </c>
-      <c r="G87" t="s">
-        <v>145</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -3514,19 +3340,10 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>293</v>
+        <v>402</v>
       </c>
       <c r="D88" t="s">
-        <v>281</v>
-      </c>
-      <c r="E88" t="s">
-        <v>59</v>
-      </c>
-      <c r="F88" t="s">
-        <v>193</v>
-      </c>
-      <c r="G88" t="s">
-        <v>146</v>
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3537,19 +3354,10 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
+        <v>403</v>
       </c>
       <c r="D89" t="s">
-        <v>281</v>
-      </c>
-      <c r="E89" t="s">
-        <v>60</v>
-      </c>
-      <c r="F89" t="s">
-        <v>193</v>
-      </c>
-      <c r="G89" t="s">
-        <v>147</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -3560,19 +3368,10 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>295</v>
+        <v>401</v>
       </c>
       <c r="D90" t="s">
-        <v>281</v>
-      </c>
-      <c r="E90" t="s">
-        <v>61</v>
-      </c>
-      <c r="F90" t="s">
-        <v>193</v>
-      </c>
-      <c r="G90" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -3583,10 +3382,10 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>425</v>
+        <v>376</v>
       </c>
       <c r="D91" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -3597,19 +3396,19 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
       <c r="D92" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E92" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F92" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="G92" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -3620,19 +3419,19 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D93" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E93" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F93" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="G93" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3643,19 +3442,19 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>299</v>
+        <v>266</v>
       </c>
       <c r="D94" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E94" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F94" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="G94" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -3666,19 +3465,19 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
       <c r="D95" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E95" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F95" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="G95" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -3689,10 +3488,10 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>386</v>
+        <v>337</v>
       </c>
       <c r="D96" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3703,10 +3502,10 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>387</v>
+        <v>338</v>
       </c>
       <c r="D97" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3717,10 +3516,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>388</v>
+        <v>339</v>
       </c>
       <c r="D98" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3731,10 +3530,10 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>389</v>
+        <v>340</v>
       </c>
       <c r="D99" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3745,10 +3544,10 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>390</v>
+        <v>341</v>
       </c>
       <c r="D100" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3759,10 +3558,10 @@
         <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>391</v>
+        <v>342</v>
       </c>
       <c r="D101" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3773,10 +3572,10 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>392</v>
+        <v>343</v>
       </c>
       <c r="D102" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3787,10 +3586,10 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>393</v>
+        <v>344</v>
       </c>
       <c r="D103" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3801,10 +3600,10 @@
         <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>394</v>
+        <v>345</v>
       </c>
       <c r="D104" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3815,10 +3614,10 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>395</v>
+        <v>346</v>
       </c>
       <c r="D105" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3829,10 +3628,10 @@
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>396</v>
+        <v>347</v>
       </c>
       <c r="D106" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3843,19 +3642,19 @@
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="D107" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E107" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F107" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="G107" t="s">
-        <v>301</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3866,19 +3665,19 @@
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>321</v>
+        <v>281</v>
       </c>
       <c r="D108" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E108" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F108" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="G108" t="s">
-        <v>302</v>
+        <v>66</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3889,22 +3688,19 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="D109" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E109" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F109" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="G109" t="s">
-        <v>303</v>
-      </c>
-      <c r="H109" t="s">
-        <v>154</v>
+        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3915,22 +3711,22 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="D110" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E110" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F110" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="G110" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="H110" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3941,19 +3737,22 @@
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="D111" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E111" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F111" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="G111" t="s">
-        <v>74</v>
+        <v>270</v>
+      </c>
+      <c r="H111" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -3964,19 +3763,19 @@
         <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="D112" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E112" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F112" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="G112" t="s">
-        <v>75</v>
+        <v>269</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
@@ -3987,19 +3786,19 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="D113" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E113" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F113" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="G113" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -4010,19 +3809,19 @@
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="D114" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E114" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F114" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="G114" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -4033,19 +3832,19 @@
         <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="D115" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E115" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F115" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="G115" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -4056,19 +3855,19 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>427</v>
+        <v>377</v>
       </c>
       <c r="D116" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E116" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F116" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="G116" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -4079,22 +3878,22 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>318</v>
+        <v>382</v>
       </c>
       <c r="D117" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E117" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F117" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="G117" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="I117" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -4105,19 +3904,19 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>319</v>
+        <v>285</v>
       </c>
       <c r="D118" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E118" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F118" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="G118" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -4128,19 +3927,19 @@
         <v>13</v>
       </c>
       <c r="C119" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
       <c r="D119" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="E119" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F119" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="G119" t="s">
-        <v>308</v>
+        <v>275</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -4151,10 +3950,10 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>397</v>
+        <v>348</v>
       </c>
       <c r="D120" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -4165,10 +3964,10 @@
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="D121" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -4179,19 +3978,19 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="D122" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="E122" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F122" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="G122" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -4202,19 +4001,19 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>437</v>
+        <v>384</v>
       </c>
       <c r="D123" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="E123" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F123" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="G123" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -4225,19 +4024,19 @@
         <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D124" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="E124" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F124" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="G124" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -4248,19 +4047,19 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D125" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="E125" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F125" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="G125" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -4271,19 +4070,19 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>438</v>
+        <v>385</v>
       </c>
       <c r="D126" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
       <c r="E126" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F126" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="G126" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -4294,19 +4093,10 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>399</v>
+        <v>350</v>
       </c>
       <c r="D127" t="s">
-        <v>322</v>
-      </c>
-      <c r="E127" t="s">
-        <v>88</v>
-      </c>
-      <c r="F127" t="s">
-        <v>193</v>
-      </c>
-      <c r="G127" t="s">
-        <v>164</v>
+        <v>288</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -4317,19 +4107,10 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>400</v>
+        <v>351</v>
       </c>
       <c r="D128" t="s">
-        <v>322</v>
-      </c>
-      <c r="E128" t="s">
-        <v>89</v>
-      </c>
-      <c r="F128" t="s">
-        <v>211</v>
-      </c>
-      <c r="G128" t="s">
-        <v>165</v>
+        <v>288</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -4340,19 +4121,10 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>401</v>
+        <v>352</v>
       </c>
       <c r="D129" t="s">
-        <v>322</v>
-      </c>
-      <c r="E129" t="s">
-        <v>90</v>
-      </c>
-      <c r="F129" t="s">
-        <v>211</v>
-      </c>
-      <c r="G129" t="s">
-        <v>166</v>
+        <v>288</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -4363,19 +4135,10 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>402</v>
+        <v>353</v>
       </c>
       <c r="D130" t="s">
-        <v>322</v>
-      </c>
-      <c r="E130" t="s">
-        <v>91</v>
-      </c>
-      <c r="F130" t="s">
-        <v>211</v>
-      </c>
-      <c r="G130" t="s">
-        <v>167</v>
+        <v>288</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -4386,10 +4149,10 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>403</v>
+        <v>354</v>
       </c>
       <c r="D131" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -4400,10 +4163,10 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>404</v>
+        <v>355</v>
       </c>
       <c r="D132" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -4414,10 +4177,10 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>405</v>
+        <v>356</v>
       </c>
       <c r="D133" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -4428,10 +4191,10 @@
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>406</v>
+        <v>357</v>
       </c>
       <c r="D134" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -4442,10 +4205,10 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>407</v>
+        <v>358</v>
       </c>
       <c r="D135" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4456,10 +4219,10 @@
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>408</v>
+        <v>359</v>
       </c>
       <c r="D136" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4470,22 +4233,22 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>338</v>
+        <v>145</v>
       </c>
       <c r="D137" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E137" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F137" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G137" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="H137" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -4496,22 +4259,22 @@
         <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>339</v>
+        <v>146</v>
       </c>
       <c r="D138" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E138" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F138" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G138" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
       <c r="H138" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -4522,22 +4285,22 @@
         <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>340</v>
+        <v>147</v>
       </c>
       <c r="D139" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E139" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F139" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G139" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
       <c r="H139" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -4548,22 +4311,22 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>341</v>
+        <v>148</v>
       </c>
       <c r="D140" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E140" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F140" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G140" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="H140" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4574,22 +4337,22 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>342</v>
+        <v>149</v>
       </c>
       <c r="D141" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E141" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F141" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G141" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
       <c r="H141" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4600,22 +4363,22 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>343</v>
+        <v>150</v>
       </c>
       <c r="D142" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E142" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F142" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="G142" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
       <c r="H142" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4626,22 +4389,22 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>350</v>
+        <v>152</v>
       </c>
       <c r="D143" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E143" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F143" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G143" t="s">
-        <v>330</v>
+        <v>297</v>
       </c>
       <c r="H143" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4652,22 +4415,22 @@
         <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>351</v>
+        <v>151</v>
       </c>
       <c r="D144" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E144" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F144" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G144" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="H144" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -4678,22 +4441,22 @@
         <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>344</v>
+        <v>153</v>
       </c>
       <c r="D145" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E145" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F145" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G145" t="s">
-        <v>332</v>
+        <v>298</v>
       </c>
       <c r="H145" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -4704,22 +4467,22 @@
         <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>345</v>
+        <v>154</v>
       </c>
       <c r="D146" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E146" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F146" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G146" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="H146" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -4730,22 +4493,22 @@
         <v>11</v>
       </c>
       <c r="C147" t="s">
-        <v>346</v>
+        <v>155</v>
       </c>
       <c r="D147" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E147" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="F147" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G147" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
       <c r="H147" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -4756,22 +4519,22 @@
         <v>12</v>
       </c>
       <c r="C148" t="s">
-        <v>347</v>
+        <v>156</v>
       </c>
       <c r="D148" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E148" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="F148" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G148" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="H148" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -4782,22 +4545,22 @@
         <v>13</v>
       </c>
       <c r="C149" t="s">
-        <v>349</v>
+        <v>157</v>
       </c>
       <c r="D149" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E149" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F149" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G149" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
       <c r="H149" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -4808,22 +4571,22 @@
         <v>14</v>
       </c>
       <c r="C150" t="s">
-        <v>348</v>
+        <v>158</v>
       </c>
       <c r="D150" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="E150" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F150" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="G150" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
       <c r="H150" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4834,10 +4597,10 @@
         <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>409</v>
+        <v>360</v>
       </c>
       <c r="D151" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4848,22 +4611,22 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>410</v>
+        <v>361</v>
       </c>
       <c r="D152" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E152" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F152" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="G152" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H152" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -4874,22 +4637,22 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>411</v>
+        <v>362</v>
       </c>
       <c r="D153" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E153" t="s">
         <v>13</v>
       </c>
       <c r="F153" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="G153" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
       <c r="H153" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -4900,22 +4663,22 @@
         <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>412</v>
+        <v>363</v>
       </c>
       <c r="D154" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E154" t="s">
         <v>11</v>
       </c>
       <c r="F154" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="G154" t="s">
-        <v>355</v>
+        <v>307</v>
       </c>
       <c r="H154" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -4926,22 +4689,22 @@
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>413</v>
+        <v>364</v>
       </c>
       <c r="D155" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E155" t="s">
         <v>12</v>
       </c>
       <c r="F155" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="G155" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="H155" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -4952,22 +4715,22 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>414</v>
+        <v>365</v>
       </c>
       <c r="D156" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E156" t="s">
         <v>15</v>
       </c>
       <c r="F156" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="G156" t="s">
-        <v>357</v>
+        <v>309</v>
       </c>
       <c r="H156" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -4978,22 +4741,22 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>415</v>
+        <v>366</v>
       </c>
       <c r="D157" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="E157" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F157" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="G157" t="s">
-        <v>358</v>
+        <v>310</v>
       </c>
       <c r="H157" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -5004,10 +4767,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
       <c r="D158" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -5018,10 +4781,10 @@
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>417</v>
+        <v>368</v>
       </c>
       <c r="D159" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -5032,10 +4795,10 @@
         <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>418</v>
+        <v>369</v>
       </c>
       <c r="D160" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,10 +4809,10 @@
         <v>10</v>
       </c>
       <c r="C161" t="s">
-        <v>419</v>
+        <v>370</v>
       </c>
       <c r="D161" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,10 +4823,10 @@
         <v>11</v>
       </c>
       <c r="C162" t="s">
-        <v>420</v>
+        <v>371</v>
       </c>
       <c r="D162" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,10 +4837,10 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>421</v>
+        <v>372</v>
       </c>
       <c r="D163" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,10 +4851,10 @@
         <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>422</v>
+        <v>373</v>
       </c>
       <c r="D164" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,10 +4865,10 @@
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>423</v>
+        <v>374</v>
       </c>
       <c r="D165" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,10 +4879,10 @@
         <v>15</v>
       </c>
       <c r="C166" t="s">
-        <v>424</v>
+        <v>375</v>
       </c>
       <c r="D166" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -5129,10 +4892,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12872662-7795-8E49-8B63-4C56A42E1535}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G9"/>
+      <selection activeCell="A2" sqref="A2:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5140,292 +4903,343 @@
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="61.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>237</v>
-      </c>
-      <c r="D3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D11" t="s">
+        <v>276</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>429</v>
-      </c>
-      <c r="D4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>183</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>430</v>
-      </c>
-      <c r="D5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C14" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>348</v>
+      </c>
+      <c r="D15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>363</v>
-      </c>
-      <c r="D6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>443</v>
-      </c>
-      <c r="D8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>190</v>
-      </c>
-      <c r="G8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>368</v>
-      </c>
-      <c r="D13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>369</v>
-      </c>
-      <c r="D14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>370</v>
-      </c>
-      <c r="D15" t="s">
-        <v>230</v>
-      </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" t="s">
-        <v>193</v>
-      </c>
-      <c r="G15" t="s">
-        <v>111</v>
+      <c r="C16" t="s">
+        <v>349</v>
+      </c>
+      <c r="D16" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`THIS IS FINAL WORKING COMMIT BEFORE I START TO DO MODIFICATION TO THE SIMULATIONS`
</commit_message>
<xml_diff>
--- a/dev/r3PGmix_info.xlsx
+++ b/dev/r3PGmix_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuk/Documents/software/r3PG/r3PGmix/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19351E6-E4F6-9B4F-A50E-4DFCC729D947}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F9D036-28B0-454E-85C1-0B10F4B11FFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28180" yWindow="460" windowWidth="18020" windowHeight="28340" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
+    <workbookView xWindow="10780" yWindow="460" windowWidth="18020" windowHeight="17540" xr2:uid="{9ECC47CC-383C-4247-B9D3-046711674009}"/>
   </bookViews>
   <sheets>
     <sheet name="var_names" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="407">
   <si>
     <t>description</t>
   </si>
@@ -1024,9 +1024,6 @@
     <t>var_4_15</t>
   </si>
   <si>
-    <t>var_5_11</t>
-  </si>
-  <si>
     <t>var_5_12</t>
   </si>
   <si>
@@ -1222,9 +1219,6 @@
     <t>var_4_11</t>
   </si>
   <si>
-    <t>var_4_8</t>
-  </si>
-  <si>
     <t>var_4_9</t>
   </si>
   <si>
@@ -1241,6 +1235,18 @@
   </si>
   <si>
     <t>var_6_11</t>
+  </si>
+  <si>
+    <t>gammaF</t>
+  </si>
+  <si>
+    <t>Litter fall rate</t>
+  </si>
+  <si>
+    <t>biom_incr_foliage</t>
+  </si>
+  <si>
+    <t>incrWF</t>
   </si>
 </sst>
 </file>
@@ -1594,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EDA796-FB5E-0A42-AB5E-6B438DB45270}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1696,7 +1702,7 @@
         <v>161</v>
       </c>
       <c r="G4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1719,7 +1725,7 @@
         <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1742,7 +1748,7 @@
         <v>160</v>
       </c>
       <c r="G6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1865,7 +1871,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D12" t="s">
         <v>189</v>
@@ -2004,7 +2010,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D20" t="s">
         <v>207</v>
@@ -2027,7 +2033,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D21" t="s">
         <v>207</v>
@@ -2096,7 +2102,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D24" t="s">
         <v>207</v>
@@ -2142,7 +2148,7 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D26" t="s">
         <v>207</v>
@@ -2156,7 +2162,7 @@
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D27" t="s">
         <v>207</v>
@@ -2170,7 +2176,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D28" t="s">
         <v>207</v>
@@ -2249,7 +2255,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D33" t="s">
         <v>220</v>
@@ -2318,7 +2324,7 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D36" t="s">
         <v>220</v>
@@ -2641,7 +2647,7 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D52" t="s">
         <v>229</v>
@@ -2661,7 +2667,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D53" t="s">
         <v>229</v>
@@ -2684,10 +2690,13 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="D54" t="s">
         <v>229</v>
+      </c>
+      <c r="G54" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2698,7 +2707,7 @@
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D55" t="s">
         <v>229</v>
@@ -2712,7 +2721,7 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D56" t="s">
         <v>229</v>
@@ -2726,7 +2735,7 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D57" t="s">
         <v>229</v>
@@ -3026,10 +3035,13 @@
         <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>332</v>
+        <v>403</v>
       </c>
       <c r="D72" t="s">
         <v>242</v>
+      </c>
+      <c r="G72" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -3040,7 +3052,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D73" t="s">
         <v>242</v>
@@ -3054,7 +3066,7 @@
         <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D74" t="s">
         <v>242</v>
@@ -3068,7 +3080,7 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D75" t="s">
         <v>242</v>
@@ -3082,7 +3094,7 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D76" t="s">
         <v>242</v>
@@ -3154,7 +3166,7 @@
         <v>178</v>
       </c>
       <c r="G79" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -3326,7 +3338,7 @@
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D87" t="s">
         <v>254</v>
@@ -3340,7 +3352,7 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D88" t="s">
         <v>254</v>
@@ -3354,7 +3366,7 @@
         <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D89" t="s">
         <v>254</v>
@@ -3368,7 +3380,7 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D90" t="s">
         <v>254</v>
@@ -3382,7 +3394,7 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D91" t="s">
         <v>254</v>
@@ -3488,7 +3500,7 @@
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D96" t="s">
         <v>134</v>
@@ -3502,7 +3514,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D97" t="s">
         <v>134</v>
@@ -3516,7 +3528,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D98" t="s">
         <v>134</v>
@@ -3530,7 +3542,7 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D99" t="s">
         <v>134</v>
@@ -3544,7 +3556,7 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D100" t="s">
         <v>134</v>
@@ -3558,7 +3570,7 @@
         <v>10</v>
       </c>
       <c r="C101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D101" t="s">
         <v>134</v>
@@ -3572,7 +3584,7 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D102" t="s">
         <v>134</v>
@@ -3586,7 +3598,7 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D103" t="s">
         <v>134</v>
@@ -3600,7 +3612,7 @@
         <v>13</v>
       </c>
       <c r="C104" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D104" t="s">
         <v>134</v>
@@ -3614,7 +3626,7 @@
         <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D105" t="s">
         <v>134</v>
@@ -3628,7 +3640,7 @@
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D106" t="s">
         <v>134</v>
@@ -3855,7 +3867,7 @@
         <v>10</v>
       </c>
       <c r="C116" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D116" t="s">
         <v>276</v>
@@ -3878,7 +3890,7 @@
         <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D117" t="s">
         <v>276</v>
@@ -3893,7 +3905,7 @@
         <v>274</v>
       </c>
       <c r="I117" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -3950,7 +3962,7 @@
         <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D120" t="s">
         <v>276</v>
@@ -3964,7 +3976,7 @@
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D121" t="s">
         <v>276</v>
@@ -3978,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D122" t="s">
         <v>288</v>
@@ -4001,7 +4013,7 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D123" t="s">
         <v>288</v>
@@ -4070,7 +4082,7 @@
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D126" t="s">
         <v>288</v>
@@ -4093,7 +4105,7 @@
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D127" t="s">
         <v>288</v>
@@ -4107,7 +4119,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D128" t="s">
         <v>288</v>
@@ -4121,7 +4133,7 @@
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D129" t="s">
         <v>288</v>
@@ -4135,7 +4147,7 @@
         <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D130" t="s">
         <v>288</v>
@@ -4149,7 +4161,7 @@
         <v>10</v>
       </c>
       <c r="C131" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D131" t="s">
         <v>288</v>
@@ -4163,7 +4175,7 @@
         <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D132" t="s">
         <v>288</v>
@@ -4177,7 +4189,7 @@
         <v>12</v>
       </c>
       <c r="C133" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D133" t="s">
         <v>288</v>
@@ -4191,7 +4203,7 @@
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D134" t="s">
         <v>288</v>
@@ -4205,7 +4217,7 @@
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D135" t="s">
         <v>288</v>
@@ -4219,7 +4231,7 @@
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D136" t="s">
         <v>288</v>
@@ -4597,7 +4609,7 @@
         <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D151" t="s">
         <v>289</v>
@@ -4611,7 +4623,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D152" t="s">
         <v>304</v>
@@ -4637,7 +4649,7 @@
         <v>2</v>
       </c>
       <c r="C153" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D153" t="s">
         <v>304</v>
@@ -4663,7 +4675,7 @@
         <v>3</v>
       </c>
       <c r="C154" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D154" t="s">
         <v>304</v>
@@ -4689,7 +4701,7 @@
         <v>4</v>
       </c>
       <c r="C155" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D155" t="s">
         <v>304</v>
@@ -4715,7 +4727,7 @@
         <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D156" t="s">
         <v>304</v>
@@ -4741,7 +4753,7 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D157" t="s">
         <v>304</v>
@@ -4767,7 +4779,7 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D158" t="s">
         <v>304</v>
@@ -4781,7 +4793,7 @@
         <v>8</v>
       </c>
       <c r="C159" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D159" t="s">
         <v>304</v>
@@ -4795,7 +4807,7 @@
         <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D160" t="s">
         <v>304</v>
@@ -4809,7 +4821,7 @@
         <v>10</v>
       </c>
       <c r="C161" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D161" t="s">
         <v>304</v>
@@ -4823,7 +4835,7 @@
         <v>11</v>
       </c>
       <c r="C162" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D162" t="s">
         <v>304</v>
@@ -4837,7 +4849,7 @@
         <v>12</v>
       </c>
       <c r="C163" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D163" t="s">
         <v>304</v>
@@ -4851,7 +4863,7 @@
         <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D164" t="s">
         <v>304</v>
@@ -4865,7 +4877,7 @@
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D165" t="s">
         <v>304</v>
@@ -4879,7 +4891,7 @@
         <v>15</v>
       </c>
       <c r="C166" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D166" t="s">
         <v>304</v>
@@ -5130,7 +5142,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D11" t="s">
         <v>276</v>
@@ -5153,7 +5165,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D12" t="s">
         <v>276</v>
@@ -5222,7 +5234,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" t="s">
         <v>276</v>
@@ -5236,7 +5248,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
         <v>276</v>

</xml_diff>